<commit_message>
ECOLI AND SCEREVISIAE SYSTEMS OPTIMIZED AND REFACTORIZED
</commit_message>
<xml_diff>
--- a/DOTS_SIMULATION/Comparativa.xlsx
+++ b/DOTS_SIMULATION/Comparativa.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IVAN\Desktop\Codes\UnityProjects\DOTS_SIMULATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4478D3BA-49A0-41FA-A812-24DA995F105C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB1B481-A990-469F-8C73-8CD37F2BD950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6933E765-E18D-4FB8-9034-0EE0E66BC137}"/>
+    <workbookView xWindow="8025" yWindow="1230" windowWidth="12840" windowHeight="11385" activeTab="1" xr2:uid="{6933E765-E18D-4FB8-9034-0EE0E66BC137}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="25">
   <si>
     <t>PRUEBA DE 1 MINUTO Y MEDIO DE DURACIÓN</t>
   </si>
@@ -78,12 +79,48 @@
   </si>
   <si>
     <t>SCEREVISIAE</t>
+  </si>
+  <si>
+    <t>CRECIMIENTO NORMAL APROXIMADO DE ECOLI Y SCEREVISIAE</t>
+  </si>
+  <si>
+    <t>ORGANISMO</t>
+  </si>
+  <si>
+    <t>CANTIDAD ESPERADA APROXIMADA</t>
+  </si>
+  <si>
+    <t>ECOLI</t>
+  </si>
+  <si>
+    <t>TIEMPO DUPLICACION APROX (min)</t>
+  </si>
+  <si>
+    <t>TIEMPO TRANSCURRIDO (min)</t>
+  </si>
+  <si>
+    <t>CANTIDAD SIMULADA</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>HORAS</t>
+  </si>
+  <si>
+    <t>MINUTOS</t>
+  </si>
+  <si>
+    <t>SEGUNDOS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000%"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -149,10 +186,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -160,6 +198,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -499,7 +540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F8242A3-EB79-4FD0-9880-73FFD20293DF}">
   <dimension ref="B1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -512,72 +553,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="J1" s="5" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="J1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="J3" s="3" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="J3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="F5" s="4" t="s">
+      <c r="C5" s="5"/>
+      <c r="F5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="J5" s="4" t="s">
+      <c r="G5" s="5"/>
+      <c r="J5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="4"/>
-      <c r="N5" s="4" t="s">
+      <c r="K5" s="5"/>
+      <c r="N5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="4"/>
+      <c r="O5" s="5"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -798,32 +839,32 @@
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="F17" s="4" t="s">
+      <c r="C17" s="5"/>
+      <c r="F17" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G17" s="4"/>
+      <c r="G17" s="5"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
@@ -946,32 +987,32 @@
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="F29" s="4" t="s">
+      <c r="C29" s="5"/>
+      <c r="F29" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G29" s="4"/>
+      <c r="G29" s="5"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
@@ -1095,11 +1136,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="J3:O4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="J1:O1"/>
     <mergeCell ref="B27:G28"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="F29:G29"/>
@@ -1109,6 +1145,148 @@
     <mergeCell ref="B15:G16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="F17:G17"/>
+    <mergeCell ref="J3:O4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="J1:O1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BF7FE7D-5952-404B-9164-88E35970AB51}">
+  <dimension ref="A4:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>38</v>
+      </c>
+      <c r="E6" s="1">
+        <v>40</v>
+      </c>
+      <c r="F6" s="1">
+        <f>(C6 * 60) + D6 + (E6 / 60)</f>
+        <v>338.66666666666669</v>
+      </c>
+      <c r="G6" s="1">
+        <v>121393</v>
+      </c>
+      <c r="H6" s="1">
+        <v>121393</v>
+      </c>
+      <c r="I6" s="3">
+        <f>ABS(G6-H6)/G6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1">
+        <v>90</v>
+      </c>
+      <c r="C7" s="1">
+        <f>C6</f>
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" ref="D7:E7" si="0">D6</f>
+        <v>38</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="F7" s="1">
+        <f>(C7 * 60) + D7 + (E7 / 60)</f>
+        <v>338.66666666666669</v>
+      </c>
+      <c r="G7" s="1">
+        <f>ROUND(EXP((F7 * LN(2)) / B7), 0)</f>
+        <v>14</v>
+      </c>
+      <c r="H7" s="1">
+        <v>13</v>
+      </c>
+      <c r="I7" s="3">
+        <f>ABS(G7-H7)/G7</f>
+        <v>7.1428571428571425E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>